<commit_message>
Fix Statistic return 0
</commit_message>
<xml_diff>
--- a/WebEnterprise-mssql/WebEnterprise-mssql.Api/~App_Data/Statistics/GetAllPostByTopic.xlsx
+++ b/WebEnterprise-mssql/WebEnterprise-mssql.Api/~App_Data/Statistics/GetAllPostByTopic.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DataName</t>
   </si>
@@ -20,7 +20,16 @@
     <t>Percent</t>
   </si>
   <si>
-    <t>jungle</t>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>test 333</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>Test567</t>
   </si>
 </sst>
 </file>
@@ -66,7 +75,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -89,7 +98,31 @@
         <v>2</v>
       </c>
       <c r="B2" s="0">
-        <v>100</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>